<commit_message>
First try at easier tables
</commit_message>
<xml_diff>
--- a/source/lore/species/Aging.xlsx
+++ b/source/lore/species/Aging.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Hobbies\TTRPG\Iuncterra\wiki\source\_assets\species\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd\Documents\GitHub\Iuncterra\source\lore\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE853DC4-B930-4DFA-B289-880FE623BFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32545E11-4BD9-44C2-BBEA-4D520D74EF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{1BE3EDDB-DCCE-4B1A-8A91-717F8D05B840}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1BE3EDDB-DCCE-4B1A-8A91-717F8D05B840}"/>
   </bookViews>
   <sheets>
     <sheet name="Lifespan" sheetId="1" r:id="rId1"/>
-    <sheet name="Multiplier" sheetId="2" r:id="rId2"/>
+    <sheet name="Elf" sheetId="3" r:id="rId2"/>
+    <sheet name="Multiplier" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Human</t>
   </si>
@@ -79,6 +80,12 @@
   </si>
   <si>
     <t>Lifespan</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Equivalent</t>
   </si>
 </sst>
 </file>
@@ -187,9 +194,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -227,7 +234,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -333,7 +340,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -475,7 +482,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -485,13 +492,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823BF021-5F91-43D9-A8D8-82E0B8EAA4AE}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="1" t="s">
         <v>12</v>
@@ -530,7 +537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -571,7 +578,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -610,7 +617,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -647,7 +654,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -668,7 +675,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -689,7 +696,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -710,7 +717,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -731,7 +738,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -752,7 +759,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -773,7 +780,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -794,7 +801,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -815,7 +822,7 @@
       </c>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -847,12 +854,215 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98299D97-A66D-4FE3-8295-5ADDAD7CF8DC}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <f>ROUNDDOWN(A2/4, 0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B21" si="0">ROUNDDOWN(A3/4, 0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>54</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>72</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>90</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>108</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>126</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>144</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>162</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>180</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>198</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>216</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>234</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>252</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>270</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>288</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>306</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>324</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>342</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>360</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8C7025-BE2C-4D73-8B2D-C56DDE8FD0F7}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>